<commit_message>
Removed leading spaces in gl names and values
</commit_message>
<xml_diff>
--- a/raw/Grand List Data revised 5-2018.xlsx
+++ b/raw/Grand List Data revised 5-2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="New Info received 2018" sheetId="1" state="visible" r:id="rId2"/>
@@ -7832,8 +7832,8 @@
   </sheetPr>
   <dimension ref="A1:I170"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D105" activeCellId="0" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27433,7 +27433,7 @@
   </sheetPr>
   <dimension ref="A1:IW174"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D37" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>

</xml_diff>